<commit_message>
Work in progress, do not pull
</commit_message>
<xml_diff>
--- a/notes/MaterialMagic.xlsx
+++ b/notes/MaterialMagic.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24780" windowHeight="9105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24780" windowHeight="9105" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="515">
   <si>
     <t>Gold Ore</t>
   </si>
@@ -1338,16 +1340,254 @@
   </si>
   <si>
     <t>structure_block</t>
+  </si>
+  <si>
+    <t>Stone</t>
+  </si>
+  <si>
+    <t>Granite</t>
+  </si>
+  <si>
+    <t>Granite_Polished</t>
+  </si>
+  <si>
+    <t>Diorite</t>
+  </si>
+  <si>
+    <t>Diorite_Polished</t>
+  </si>
+  <si>
+    <t>Andesite</t>
+  </si>
+  <si>
+    <t>Andesite_Polished</t>
+  </si>
+  <si>
+    <t>Dirt</t>
+  </si>
+  <si>
+    <t>Dirt_Coarse</t>
+  </si>
+  <si>
+    <t>Podzol</t>
+  </si>
+  <si>
+    <t>Sand</t>
+  </si>
+  <si>
+    <t>Sand_Red</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Wood_Oak</t>
+  </si>
+  <si>
+    <t>Wood_Spruce</t>
+  </si>
+  <si>
+    <t>Wood_Birch</t>
+  </si>
+  <si>
+    <t>Wood_Jungle</t>
+  </si>
+  <si>
+    <t>Wood_Acacia</t>
+  </si>
+  <si>
+    <t>Wood_Dark_Oak</t>
+  </si>
+  <si>
+    <t>(direction)</t>
+  </si>
+  <si>
+    <t>Wool</t>
+  </si>
+  <si>
+    <t>Wool_colors</t>
+  </si>
+  <si>
+    <t>Clay_colors</t>
+  </si>
+  <si>
+    <t>Glass_colors</t>
+  </si>
+  <si>
+    <t>Slab</t>
+  </si>
+  <si>
+    <t>Slab_Stone</t>
+  </si>
+  <si>
+    <t>DoubleSlab</t>
+  </si>
+  <si>
+    <t>DoubleSlab_Stone</t>
+  </si>
+  <si>
+    <t>DoubleSlab_Cobblestone</t>
+  </si>
+  <si>
+    <t>DoubleSlab_Bricks</t>
+  </si>
+  <si>
+    <t>DoubleSlab_StoneWood</t>
+  </si>
+  <si>
+    <t>DoubleSlab_Stone_Bricks</t>
+  </si>
+  <si>
+    <t>DoubleSlab_Nether_Bricks</t>
+  </si>
+  <si>
+    <t>DoubleSlab_Quartz</t>
+  </si>
+  <si>
+    <t>DoubleSlab_Stone_Smooth</t>
+  </si>
+  <si>
+    <t>DoubleSlab_Sandstone</t>
+  </si>
+  <si>
+    <t>Quartz</t>
+  </si>
+  <si>
+    <t>Sandstone</t>
+  </si>
+  <si>
+    <t>Slab_StoneWood</t>
+  </si>
+  <si>
+    <t>Slab_Cobblestone</t>
+  </si>
+  <si>
+    <t>Slab_Bricks</t>
+  </si>
+  <si>
+    <t>Slab_Stone_Bricks</t>
+  </si>
+  <si>
+    <t>Slab_Nether_Bricks</t>
+  </si>
+  <si>
+    <t>Slab_Quartz</t>
+  </si>
+  <si>
+    <t>DoubleSlab_Sandstone_Red</t>
+  </si>
+  <si>
+    <t>DoubleSlab_Sandstone_Red_Smooth</t>
+  </si>
+  <si>
+    <t>Slab_Sandstone_Red</t>
+  </si>
+  <si>
+    <t>DoubleSlab_Quartz_Tile</t>
+  </si>
+  <si>
+    <t>Slab_Stone_Upper</t>
+  </si>
+  <si>
+    <t>Slab_StoneWood_Upper</t>
+  </si>
+  <si>
+    <t>Slab_Cobblestone_Upper</t>
+  </si>
+  <si>
+    <t>Slab_Bricks_Upper</t>
+  </si>
+  <si>
+    <t>Slab_Stone_Bricks_Upper</t>
+  </si>
+  <si>
+    <t>Slab_Nether_Bricks_Upper</t>
+  </si>
+  <si>
+    <t>Slab_Quartz_Upper</t>
+  </si>
+  <si>
+    <t>Slab_Sandstone_Red_Upper</t>
+  </si>
+  <si>
+    <t>Sandstone_Chiseled</t>
+  </si>
+  <si>
+    <t>Sandstone_Smooth</t>
+  </si>
+  <si>
+    <t>Sandstone_Red</t>
+  </si>
+  <si>
+    <t>Sandstone_Red_Chiseled</t>
+  </si>
+  <si>
+    <t>Sandstone_Red_Smooth</t>
+  </si>
+  <si>
+    <t>Stonebrick</t>
+  </si>
+  <si>
+    <t>Stonebrick_Mossy</t>
+  </si>
+  <si>
+    <t>Stonebrick_Cracked</t>
+  </si>
+  <si>
+    <t>Stonebrick_Chiseled</t>
+  </si>
+  <si>
+    <t>Prismarine</t>
+  </si>
+  <si>
+    <t>Prismarine_Bricks</t>
+  </si>
+  <si>
+    <t>Prismarine_Dark</t>
+  </si>
+  <si>
+    <t>Sponge</t>
+  </si>
+  <si>
+    <t>Sponge_Wet</t>
+  </si>
+  <si>
+    <t>Cobblestone_Wall</t>
+  </si>
+  <si>
+    <t>Cobblestone_Mossy_Wall</t>
+  </si>
+  <si>
+    <t>Quartz_Chiseled</t>
+  </si>
+  <si>
+    <t>Quartz_Pillar</t>
+  </si>
+  <si>
+    <t>Quartz_Pillar_UD</t>
+  </si>
+  <si>
+    <t>Quartz_Pillar_NS</t>
+  </si>
+  <si>
+    <t>Quartz_Pillar_EW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1373,13 +1613,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1387,16 +1628,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1722,8 +1953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6995,7 +7226,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7007,4 +7238,294 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="15" width="18.25" customWidth="1"/>
+    <col min="17" max="17" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B1" t="s">
+        <v>445</v>
+      </c>
+      <c r="C1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D1" t="s">
+        <v>450</v>
+      </c>
+      <c r="E1" t="s">
+        <v>458</v>
+      </c>
+      <c r="F1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>464</v>
+      </c>
+      <c r="I1" t="s">
+        <v>475</v>
+      </c>
+      <c r="J1" t="s">
+        <v>496</v>
+      </c>
+      <c r="K1" t="s">
+        <v>499</v>
+      </c>
+      <c r="L1" t="s">
+        <v>503</v>
+      </c>
+      <c r="M1" t="s">
+        <v>506</v>
+      </c>
+      <c r="N1" t="s">
+        <v>508</v>
+      </c>
+      <c r="O1" t="s">
+        <v>474</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>439</v>
+      </c>
+      <c r="B2" t="s">
+        <v>446</v>
+      </c>
+      <c r="C2" t="s">
+        <v>449</v>
+      </c>
+      <c r="D2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E2" t="s">
+        <v>459</v>
+      </c>
+      <c r="F2" t="s">
+        <v>460</v>
+      </c>
+      <c r="G2" t="s">
+        <v>461</v>
+      </c>
+      <c r="H2" t="s">
+        <v>465</v>
+      </c>
+      <c r="I2" t="s">
+        <v>494</v>
+      </c>
+      <c r="J2" t="s">
+        <v>497</v>
+      </c>
+      <c r="K2" t="s">
+        <v>500</v>
+      </c>
+      <c r="L2" t="s">
+        <v>504</v>
+      </c>
+      <c r="M2" t="s">
+        <v>507</v>
+      </c>
+      <c r="N2" t="s">
+        <v>509</v>
+      </c>
+      <c r="O2" t="s">
+        <v>510</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>440</v>
+      </c>
+      <c r="B3" t="s">
+        <v>447</v>
+      </c>
+      <c r="D3" t="s">
+        <v>452</v>
+      </c>
+      <c r="H3" t="s">
+        <v>468</v>
+      </c>
+      <c r="I3" t="s">
+        <v>495</v>
+      </c>
+      <c r="J3" t="s">
+        <v>498</v>
+      </c>
+      <c r="K3" t="s">
+        <v>501</v>
+      </c>
+      <c r="L3" t="s">
+        <v>505</v>
+      </c>
+      <c r="O3" t="s">
+        <v>511</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>441</v>
+      </c>
+      <c r="D4" t="s">
+        <v>453</v>
+      </c>
+      <c r="H4" t="s">
+        <v>466</v>
+      </c>
+      <c r="K4" t="s">
+        <v>502</v>
+      </c>
+      <c r="O4" t="s">
+        <v>512</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>442</v>
+      </c>
+      <c r="D5" t="s">
+        <v>454</v>
+      </c>
+      <c r="H5" t="s">
+        <v>467</v>
+      </c>
+      <c r="O5" t="s">
+        <v>513</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>443</v>
+      </c>
+      <c r="D6" t="s">
+        <v>455</v>
+      </c>
+      <c r="H6" t="s">
+        <v>469</v>
+      </c>
+      <c r="O6" t="s">
+        <v>514</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>444</v>
+      </c>
+      <c r="D7" t="s">
+        <v>456</v>
+      </c>
+      <c r="H7" t="s">
+        <v>470</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>457</v>
+      </c>
+      <c r="H8" t="s">
+        <v>471</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>472</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>473</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>482</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>483</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q14" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q15" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q16" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="17" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q17" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>